<commit_message>
clocked in and out btn state
</commit_message>
<xml_diff>
--- a/django-hrms-project-plan.xlsx
+++ b/django-hrms-project-plan.xlsx
@@ -158,6 +158,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -179,6 +180,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -296,11 +298,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.5612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>